<commit_message>
sua duong link truy cap trang admin
</commit_message>
<xml_diff>
--- a/PhanChiaCongViec.xlsx
+++ b/PhanChiaCongViec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CYBERSOFT\_9_REACTJS\Bài tập CapStone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\BC32E_PhuongDuDucThe_NguyenDoanTruongVi_Capstone_MovieBookingProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -319,9 +319,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -337,15 +334,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -362,49 +350,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -435,44 +399,47 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -712,679 +679,679 @@
   <dimension ref="A1:L992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.25" style="16" customWidth="1"/>
-    <col min="2" max="2" width="19.125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="16" customWidth="1"/>
-    <col min="4" max="4" width="10.625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.375" style="16" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="21.625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="9.25" style="16" customWidth="1"/>
-    <col min="10" max="10" width="7.625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="21.5" style="16" customWidth="1"/>
-    <col min="12" max="12" width="33" style="16" customWidth="1"/>
-    <col min="13" max="28" width="7.625" style="16" customWidth="1"/>
-    <col min="29" max="16384" width="12.625" style="16"/>
+    <col min="1" max="1" width="9.25" style="12" customWidth="1"/>
+    <col min="2" max="2" width="19.125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="7.625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="21.625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="9.25" style="12" customWidth="1"/>
+    <col min="10" max="10" width="7.625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="21.5" style="12" customWidth="1"/>
+    <col min="12" max="12" width="33" style="12" customWidth="1"/>
+    <col min="13" max="28" width="7.625" style="12" customWidth="1"/>
+    <col min="29" max="16384" width="12.625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:12" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11">
+      <c r="C2" s="33"/>
+      <c r="D2" s="7">
         <v>44847</v>
       </c>
-      <c r="E2" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F2" s="12">
-        <v>1</v>
-      </c>
-      <c r="G2" s="13" t="s">
+      <c r="E2" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="10">
         <v>44870</v>
       </c>
-      <c r="I2" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J2" s="12">
-        <v>1</v>
-      </c>
-      <c r="K2" s="13" t="s">
+      <c r="I2" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="15"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="11">
+      <c r="A3" s="36"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="7">
         <v>44847</v>
       </c>
-      <c r="E3" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="E3" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="10">
         <v>44870</v>
       </c>
-      <c r="I3" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J3" s="12">
-        <v>1</v>
-      </c>
-      <c r="K3" s="13" t="s">
+      <c r="I3" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J3" s="8">
+        <v>1</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="15"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="11">
+      <c r="A4" s="36"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="7">
         <v>44847</v>
       </c>
-      <c r="E4" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="E4" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="10">
         <v>44870</v>
       </c>
-      <c r="I4" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J4" s="12">
-        <v>1</v>
-      </c>
-      <c r="K4" s="13" t="s">
+      <c r="I4" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J4" s="8">
+        <v>1</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="15"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="11">
+      <c r="A5" s="36"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="7">
         <v>44847</v>
       </c>
-      <c r="E5" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F5" s="12">
-        <v>1</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="E5" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="10">
         <v>44870</v>
       </c>
-      <c r="I5" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J5" s="12">
-        <v>1</v>
-      </c>
-      <c r="K5" s="13" t="s">
+      <c r="I5" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="15"/>
+      <c r="L5" s="11"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="11">
+      <c r="A6" s="36"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="7">
         <v>44847</v>
       </c>
-      <c r="E6" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F6" s="12">
-        <v>1</v>
-      </c>
-      <c r="G6" s="13" t="s">
+      <c r="E6" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="10">
         <v>44870</v>
       </c>
-      <c r="I6" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J6" s="12">
-        <v>1</v>
-      </c>
-      <c r="K6" s="13" t="s">
+      <c r="I6" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" ht="9" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="11">
+      <c r="A7" s="36"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="7">
         <v>44847</v>
       </c>
-      <c r="E7" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13" t="s">
+      <c r="E7" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="10">
         <v>44870</v>
       </c>
-      <c r="I7" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J7" s="12">
-        <v>1</v>
-      </c>
-      <c r="K7" s="13" t="s">
+      <c r="I7" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11">
+      <c r="C8" s="33"/>
+      <c r="D8" s="7">
         <v>44847</v>
       </c>
-      <c r="E8" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F8" s="12">
-        <v>1</v>
-      </c>
-      <c r="G8" s="13" t="s">
+      <c r="E8" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="10">
         <v>44870</v>
       </c>
-      <c r="I8" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J8" s="12">
-        <v>1</v>
-      </c>
-      <c r="K8" s="13" t="s">
+      <c r="I8" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="15"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="36"/>
+      <c r="B9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11">
+      <c r="C9" s="33"/>
+      <c r="D9" s="7">
         <v>44847</v>
       </c>
-      <c r="E9" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F9" s="12">
-        <v>1</v>
-      </c>
-      <c r="G9" s="13" t="s">
+      <c r="E9" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="10">
         <v>44870</v>
       </c>
-      <c r="I9" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J9" s="12">
-        <v>1</v>
-      </c>
-      <c r="K9" s="13" t="s">
+      <c r="I9" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="15"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11">
+      <c r="C10" s="33"/>
+      <c r="D10" s="7">
         <v>44847</v>
       </c>
-      <c r="E10" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F10" s="12">
-        <v>1</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="E10" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="10">
         <v>44870</v>
       </c>
-      <c r="I10" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J10" s="12">
-        <v>1</v>
-      </c>
-      <c r="K10" s="13" t="s">
+      <c r="I10" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J10" s="8">
+        <v>1</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="15"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="7">
         <v>44847</v>
       </c>
-      <c r="E11" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F11" s="12">
-        <v>1</v>
-      </c>
-      <c r="G11" s="13" t="s">
+      <c r="E11" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="10">
         <v>44870</v>
       </c>
-      <c r="I11" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J11" s="12">
-        <v>1</v>
-      </c>
-      <c r="K11" s="13" t="s">
+      <c r="I11" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="15"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="7">
         <v>44847</v>
       </c>
-      <c r="E12" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F12" s="12">
-        <v>1</v>
-      </c>
-      <c r="G12" s="13" t="s">
+      <c r="E12" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="10">
         <v>44870</v>
       </c>
-      <c r="I12" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J12" s="12">
-        <v>1</v>
-      </c>
-      <c r="K12" s="13" t="s">
+      <c r="I12" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J12" s="8">
+        <v>1</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="15"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="7">
         <v>44847</v>
       </c>
-      <c r="E13" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F13" s="12">
-        <v>1</v>
-      </c>
-      <c r="G13" s="13" t="s">
+      <c r="E13" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="10">
         <v>44870</v>
       </c>
-      <c r="I13" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J13" s="12">
-        <v>1</v>
-      </c>
-      <c r="K13" s="13" t="s">
+      <c r="I13" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1</v>
+      </c>
+      <c r="K13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="15"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="7">
         <v>44847</v>
       </c>
-      <c r="E14" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F14" s="12">
-        <v>1</v>
-      </c>
-      <c r="G14" s="13" t="s">
+      <c r="E14" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="10">
         <v>44870</v>
       </c>
-      <c r="I14" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J14" s="12">
-        <v>1</v>
-      </c>
-      <c r="K14" s="13" t="s">
+      <c r="I14" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J14" s="8">
+        <v>1</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="15"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="27" t="s">
+      <c r="A15" s="36"/>
+      <c r="B15" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="7">
         <v>44847</v>
       </c>
-      <c r="E15" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F15" s="12">
-        <v>1</v>
-      </c>
-      <c r="G15" s="13" t="s">
+      <c r="E15" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="10">
         <v>44870</v>
       </c>
-      <c r="I15" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J15" s="12">
-        <v>1</v>
-      </c>
-      <c r="K15" s="13" t="s">
+      <c r="I15" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J15" s="8">
+        <v>1</v>
+      </c>
+      <c r="K15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="15"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="7">
         <v>44847</v>
       </c>
-      <c r="E16" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F16" s="12">
-        <v>1</v>
-      </c>
-      <c r="G16" s="13" t="s">
+      <c r="E16" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="10">
         <v>44870</v>
       </c>
-      <c r="I16" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J16" s="12">
-        <v>1</v>
-      </c>
-      <c r="K16" s="13" t="s">
+      <c r="I16" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J16" s="8">
+        <v>1</v>
+      </c>
+      <c r="K16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="15"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32" t="s">
+      <c r="A17" s="37"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="7">
         <v>44847</v>
       </c>
-      <c r="E17" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F17" s="12">
-        <v>1</v>
-      </c>
-      <c r="G17" s="13" t="s">
+      <c r="E17" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="10">
         <v>44870</v>
       </c>
-      <c r="I17" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J17" s="12">
-        <v>1</v>
-      </c>
-      <c r="K17" s="13" t="s">
+      <c r="I17" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J17" s="8">
+        <v>1</v>
+      </c>
+      <c r="K17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="15"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11">
+      <c r="C18" s="33"/>
+      <c r="D18" s="7">
         <v>44847</v>
       </c>
-      <c r="E18" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F18" s="12">
-        <v>1</v>
-      </c>
-      <c r="G18" s="34" t="s">
+      <c r="E18" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="10">
         <v>44870</v>
       </c>
-      <c r="I18" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J18" s="12">
-        <v>1</v>
-      </c>
-      <c r="K18" s="34" t="s">
+      <c r="I18" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J18" s="8">
+        <v>1</v>
+      </c>
+      <c r="K18" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="L18" s="33"/>
+      <c r="L18" s="21"/>
     </row>
     <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11">
+      <c r="C19" s="33"/>
+      <c r="D19" s="7">
         <v>44847</v>
       </c>
-      <c r="E19" s="11">
-        <v>44874</v>
-      </c>
-      <c r="F19" s="12">
-        <v>1</v>
-      </c>
-      <c r="G19" s="34" t="s">
+      <c r="E19" s="7">
+        <v>44874</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="10">
         <v>44870</v>
       </c>
-      <c r="I19" s="14">
-        <v>44874</v>
-      </c>
-      <c r="J19" s="12">
-        <v>1</v>
-      </c>
-      <c r="K19" s="34" t="s">
+      <c r="I19" s="10">
+        <v>44874</v>
+      </c>
+      <c r="J19" s="8">
+        <v>1</v>
+      </c>
+      <c r="K19" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="33"/>
+      <c r="L19" s="21"/>
     </row>
-    <row r="20" spans="1:12" s="35" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="42"/>
+    <row r="20" spans="1:12" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="30"/>
     </row>
-    <row r="21" spans="1:12" s="35" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="35" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="42"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="30"/>
     </row>
-    <row r="22" spans="1:12" s="35" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="12"/>
+      <c r="D22" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="42"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="30"/>
     </row>
     <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2371,7 +2338,7 @@
     <mergeCell ref="B10:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="J20 F2:F22">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>